<commit_message>
beta for multiple body parts
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -8,19 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\wataru\jupyter\dlc2_edit_labels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFEF20A4-A8A1-408E-B8A1-7366099EB643}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA6D5734-F457-44AC-A5DB-E00236DC1424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-43752" yWindow="372" windowWidth="21456" windowHeight="19944" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-37170" yWindow="3120" windowWidth="24180" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
   <si>
     <t>inferred_path</t>
   </si>
@@ -92,6 +103,18 @@
   </si>
   <si>
     <t>comments</t>
+  </si>
+  <si>
+    <t>W:\wataru\dlc_data\homecage_test03-wi-2022-06-08\labeled-data\rpicam-01_1806_20210722_212134</t>
+  </si>
+  <si>
+    <t>add spine</t>
+  </si>
+  <si>
+    <t>spine1,spine2,tail1,tail2</t>
+  </si>
+  <si>
+    <t>W:\wataru\dlc_data\homecage_test04-wi-2022-06-08\labeled-data\rpicam-01_1806_20210722_212134</t>
   </si>
 </sst>
 </file>
@@ -941,29 +964,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="2" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.21875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="14.77734375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="25.21875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="29.21875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.1796875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="14.81640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="25.1796875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="29.1796875" style="2" customWidth="1"/>
     <col min="7" max="7" width="20" style="2" customWidth="1"/>
-    <col min="8" max="8" width="22.44140625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="23.44140625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="10.21875" style="3" customWidth="1"/>
-    <col min="11" max="11" width="8.88671875" style="3"/>
-    <col min="12" max="16384" width="8.88671875" style="2"/>
+    <col min="8" max="8" width="22.453125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="23.453125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="10.1796875" style="3" customWidth="1"/>
+    <col min="11" max="11" width="8.90625" style="3"/>
+    <col min="12" max="16384" width="8.90625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>21</v>
       </c>
@@ -992,7 +1016,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -1008,7 +1032,7 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="87" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -1033,7 +1057,7 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -1049,7 +1073,7 @@
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -1065,7 +1089,7 @@
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="87" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -1087,7 +1111,7 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="87" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -1097,6 +1121,9 @@
       <c r="C7" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="D7" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="G7" s="2" t="s">
         <v>7</v>
       </c>
@@ -1105,6 +1132,53 @@
       </c>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="1:11" ht="87" x14ac:dyDescent="0.35">
+      <c r="A8" s="2">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K8" s="2"/>
+    </row>
+    <row r="9" spans="1:11" ht="87" x14ac:dyDescent="0.35">
+      <c r="A9" s="2">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>